<commit_message>
added key logger to steal your shit
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Blake</t>
   </si>
@@ -76,6 +76,18 @@
   </si>
   <si>
     <t>your mom</t>
+  </si>
+  <si>
+    <t>714-943-9606</t>
+  </si>
+  <si>
+    <t>714-555-5555</t>
+  </si>
+  <si>
+    <t>555-555-5555</t>
+  </si>
+  <si>
+    <t>714-444-4444</t>
   </si>
 </sst>
 </file>
@@ -428,7 +440,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -450,8 +462,8 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1">
-        <v>7149439606</v>
+      <c r="D1" t="s">
+        <v>20</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -470,8 +482,8 @@
       <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="D2">
-        <v>7145555555</v>
+      <c r="D2" t="s">
+        <v>21</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>8</v>
@@ -490,8 +502,8 @@
       <c r="C3" t="s">
         <v>12</v>
       </c>
-      <c r="D3">
-        <v>5555555555</v>
+      <c r="D3" t="s">
+        <v>22</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>13</v>
@@ -510,8 +522,8 @@
       <c r="C4" t="s">
         <v>16</v>
       </c>
-      <c r="D4">
-        <v>4444444</v>
+      <c r="D4" t="s">
+        <v>23</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>17</v>

</xml_diff>